<commit_message>
Updated README and MIPI_deployment.xlsx
</commit_message>
<xml_diff>
--- a/MIPI_deployment.xlsx
+++ b/MIPI_deployment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\home\germaine\work\external_drive\jetson\l4t_eg\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cyril.germaine\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F34239B7-3CD0-43C9-86A0-DA429DC43A3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{893F7E93-5683-4D6A-A658-125C2CD91872}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="360" windowWidth="25440" windowHeight="15390" activeTab="1" xr2:uid="{D61E0E21-A3C2-41B9-A323-5A81E21B33EC}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{D61E0E21-A3C2-41B9-A323-5A81E21B33EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Jetson" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="40">
   <si>
     <t>System On Module</t>
   </si>
@@ -82,10 +82,6 @@
   <si>
     <t>JetPack 5.1.3
 L4T 35.5.0</t>
-  </si>
-  <si>
-    <t>JetPack 6.0
-L4T 36.3</t>
   </si>
   <si>
     <t>Dione 640/1280</t>
@@ -115,13 +111,6 @@
   </si>
   <si>
     <t>* GitHub repo for Yocto : https://github.com/xenicsir/dione_mipi_tegra/tree/main/yocto</t>
-  </si>
-  <si>
-    <t>Jetson Xavier</t>
-  </si>
-  <si>
-    <t>Jetson AGX Orin
-Auvidea X230D</t>
   </si>
   <si>
     <t>CSI Connector type</t>
@@ -163,6 +152,30 @@
   </si>
   <si>
     <t>Not supported</t>
+  </si>
+  <si>
+    <t>Jetson Orin NX devkit</t>
+  </si>
+  <si>
+    <t>Jetson Xavier NX devkit</t>
+  </si>
+  <si>
+    <t>Jetson Nano devkit</t>
+  </si>
+  <si>
+    <t>Jetson AGX Orin /
+Auvidea X230D carrier board</t>
+  </si>
+  <si>
+    <t>Jetson Orin NX</t>
+  </si>
+  <si>
+    <t>- Waveshare JETSON-ORIN-NX-DEV-KIT
+- Nvidia Orin Nano devkit</t>
+  </si>
+  <si>
+    <t>JetPack 6.2
+L4T 36.4.3</t>
   </si>
 </sst>
 </file>
@@ -281,9 +294,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -307,6 +317,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -338,7 +351,7 @@
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>86898</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>172133</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -736,10 +749,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B889CEB-6ACC-47C4-9199-C4DCCE542BFC}">
-  <dimension ref="A1:N20"/>
+  <dimension ref="A1:R20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -750,78 +763,92 @@
     <col min="4" max="4" width="10" style="1" customWidth="1"/>
     <col min="5" max="5" width="7.5703125" style="1" customWidth="1"/>
     <col min="6" max="6" width="8" style="1" customWidth="1"/>
-    <col min="7" max="8" width="7.5703125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="7.28515625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="7.5703125" style="1" customWidth="1"/>
     <col min="9" max="10" width="7.7109375" style="1" customWidth="1"/>
     <col min="11" max="11" width="8.42578125" style="1" customWidth="1"/>
     <col min="12" max="12" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="8.28515625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="10.85546875" style="1" customWidth="1"/>
-    <col min="15" max="15" width="8" style="1" customWidth="1"/>
-    <col min="16" max="16" width="11" style="1" customWidth="1"/>
-    <col min="17" max="17" width="13.85546875" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="11.42578125" style="1"/>
+    <col min="14" max="14" width="8.85546875" style="1" customWidth="1"/>
+    <col min="15" max="15" width="8.42578125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.28515625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="8.85546875" style="1" customWidth="1"/>
+    <col min="19" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17" t="s">
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17" t="s">
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16"/>
     </row>
-    <row r="2" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17" t="s">
+      <c r="B2" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="L2" s="17"/>
-      <c r="M2" s="17"/>
-      <c r="N2" s="17"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="16"/>
+      <c r="N2" s="16"/>
+      <c r="O2" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="P2" s="16"/>
+      <c r="Q2" s="16"/>
+      <c r="R2" s="16"/>
     </row>
-    <row r="3" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>7</v>
@@ -851,116 +878,152 @@
         <v>12</v>
       </c>
       <c r="N3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>13</v>
       </c>
+      <c r="B4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="R4" s="5" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="4" spans="1:14" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="5" t="s">
+    <row r="5" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="K4" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="L4" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="M4" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>35</v>
+      <c r="B5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="R5" s="5" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="K5" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="L5" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="M5" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>35</v>
-      </c>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="15"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="16"/>
-      <c r="L6" s="16"/>
-      <c r="M6" s="16"/>
-      <c r="N6" s="16"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -975,22 +1038,28 @@
       <c r="L7" s="4"/>
       <c r="M7" s="4"/>
       <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="4"/>
+      <c r="R7" s="4"/>
     </row>
-    <row r="8" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="17" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="18" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="19" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="20" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="9">
+    <mergeCell ref="O1:R1"/>
+    <mergeCell ref="O2:R2"/>
     <mergeCell ref="A6:N6"/>
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="K1:N1"/>
@@ -1008,75 +1077,89 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DCCCDB1-1EA5-4151-AA8C-0720347F41D2}">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" style="13" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" style="18" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" style="12" customWidth="1"/>
     <col min="3" max="3" width="21.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="6"/>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="D1" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="7" t="s">
+    </row>
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>28</v>
       </c>
+      <c r="D4" s="8" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="C5" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>26</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="24" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D24" s="14" t="s">
-        <v>32</v>
+      <c r="D24" s="13" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1089,12 +1172,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="ddfcbff1-988c-4780-af66-42272a7444f2" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5eab2033-26a9-4886-8f5a-efa3f46bf7e3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <SharedWithUsers xmlns="ddfcbff1-988c-4780-af66-42272a7444f2">
+      <UserInfo>
+        <DisplayName>Cyril Germaine</DisplayName>
+        <AccountId>370</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1353,27 +1445,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="ddfcbff1-988c-4780-af66-42272a7444f2" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5eab2033-26a9-4886-8f5a-efa3f46bf7e3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <SharedWithUsers xmlns="ddfcbff1-988c-4780-af66-42272a7444f2">
-      <UserInfo>
-        <DisplayName>Cyril Germaine</DisplayName>
-        <AccountId>370</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{21273CB7-CC8A-48C1-BA2A-0CD67C70C578}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C6CC26F4-9ACA-496B-B719-4372C9693134}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="5eab2033-26a9-4886-8f5a-efa3f46bf7e3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="ddfcbff1-988c-4780-af66-42272a7444f2"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1398,18 +1490,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C6CC26F4-9ACA-496B-B719-4372C9693134}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{21273CB7-CC8A-48C1-BA2A-0CD67C70C578}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="5eab2033-26a9-4886-8f5a-efa3f46bf7e3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="ddfcbff1-988c-4780-af66-42272a7444f2"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated MIPI_deployment.xlsx and README.md files
</commit_message>
<xml_diff>
--- a/MIPI_deployment.xlsx
+++ b/MIPI_deployment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cyril.germaine\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E39D1B7E-89F6-4438-8BE2-6BD39BC1B2F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{944E98FE-0335-4CCC-B6DD-B0A810DF6A8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{D61E0E21-A3C2-41B9-A323-5A81E21B33EC}"/>
   </bookViews>
@@ -174,22 +174,8 @@
 L4T 36.4.3</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">- Waveshare JETSON-ORIN-NX-DEV-KIT
-- Nvidia Orin Nano devkit
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>*CAM0 port does not work</t>
-    </r>
+    <t>- Waveshare JETSON-ORIN-NX-DEV-KIT
+- Nvidia Orin Nano devkit</t>
   </si>
 </sst>
 </file>
@@ -766,7 +752,7 @@
   <dimension ref="A1:R20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1186,6 +1172,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="ddfcbff1-988c-4780-af66-42272a7444f2" xsi:nil="true"/>
@@ -1201,15 +1196,6 @@
     </SharedWithUsers>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1468,6 +1454,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{21273CB7-CC8A-48C1-BA2A-0CD67C70C578}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C6CC26F4-9ACA-496B-B719-4372C9693134}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="5eab2033-26a9-4886-8f5a-efa3f46bf7e3"/>
@@ -1480,14 +1474,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{21273CB7-CC8A-48C1-BA2A-0CD67C70C578}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Updated MIPI_deployment.xlsx and README.md files for 1.0.3 tag
</commit_message>
<xml_diff>
--- a/MIPI_deployment.xlsx
+++ b/MIPI_deployment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cyril.germaine\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{944E98FE-0335-4CCC-B6DD-B0A810DF6A8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFE8C261-598D-48BE-90DF-245AFB7E0D6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{D61E0E21-A3C2-41B9-A323-5A81E21B33EC}"/>
   </bookViews>
@@ -37,39 +37,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
   <si>
     <t>System On Module</t>
   </si>
   <si>
-    <t>Jetson Nano</t>
-  </si>
-  <si>
-    <t>Jetson Xavier NX 16GB commercial (no SD card)</t>
-  </si>
-  <si>
-    <t>Jetson AGX Orin</t>
-  </si>
-  <si>
     <t>Carrier boards</t>
   </si>
   <si>
-    <t>Auvidea X230D</t>
-  </si>
-  <si>
     <t>Operating system version</t>
-  </si>
-  <si>
-    <t>JetPack 4.6.1
-L4T 32.7.1</t>
-  </si>
-  <si>
-    <t>JetPack 4.6.4
-L4T 32.7.4</t>
-  </si>
-  <si>
-    <t>JetPack 5.0.2
-L4T 35.1</t>
   </si>
   <si>
     <t>JetPack 5.1.1
@@ -85,9 +61,6 @@
   </si>
   <si>
     <t>Dione 640/1280</t>
-  </si>
-  <si>
-    <t>OK*</t>
   </si>
   <si>
     <t>OK</t>
@@ -96,21 +69,6 @@
     <t>MicroCube640
 SmartIR640
 Crius1280</t>
-  </si>
-  <si>
-    <t>Yocto
-L4T 32.7.1</t>
-  </si>
-  <si>
-    <t>Yocto
-L4T 32.6.1</t>
-  </si>
-  <si>
-    <t>Yocto
-L4T 32.5.1</t>
-  </si>
-  <si>
-    <t>* GitHub repo for Yocto : https://github.com/xenicsir/dione_mipi_tegra/tree/main/yocto</t>
   </si>
   <si>
     <t>CSI Connector type</t>
@@ -142,13 +100,6 @@
   </si>
   <si>
     <t>38237 Auvidea | Mouser France</t>
-  </si>
-  <si>
-    <t>- Waveshare JETSON-IO-BASE-B
-- Seeed A206 carrier board</t>
-  </si>
-  <si>
-    <t>Jetson Nano Developer Kit</t>
   </si>
   <si>
     <t>Not supported</t>
@@ -267,7 +218,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -309,17 +260,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -749,324 +697,122 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B889CEB-6ACC-47C4-9199-C4DCCE542BFC}">
-  <dimension ref="A1:R20"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10" style="1" customWidth="1"/>
-    <col min="5" max="5" width="7.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8" style="1" customWidth="1"/>
-    <col min="7" max="7" width="7.28515625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="7.5703125" style="1" customWidth="1"/>
-    <col min="9" max="10" width="7.7109375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="8.42578125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.28515625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="8.85546875" style="1" customWidth="1"/>
-    <col min="15" max="15" width="8.42578125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.28515625" style="1" customWidth="1"/>
-    <col min="18" max="18" width="8.85546875" style="1" customWidth="1"/>
-    <col min="19" max="16384" width="11.42578125" style="1"/>
+    <col min="2" max="2" width="8.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+    </row>
+    <row r="2" spans="1:5" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15" t="s">
+      <c r="B2" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+    </row>
+    <row r="3" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15" t="s">
+      <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="P1" s="15"/>
-      <c r="Q1" s="15"/>
-      <c r="R1" s="15"/>
+      <c r="C3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="2" spans="1:18" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="L2" s="15"/>
-      <c r="M2" s="15"/>
-      <c r="N2" s="15"/>
-      <c r="O2" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="P2" s="15"/>
-      <c r="Q2" s="15"/>
-      <c r="R2" s="15"/>
+    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="3" spans="1:18" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="2" t="s">
+    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="2" t="s">
+      <c r="C5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>38</v>
-      </c>
     </row>
-    <row r="4" spans="1:18" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="K4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="L4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="M4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="P4" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q4" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="R4" s="5" t="s">
-        <v>15</v>
-      </c>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="15"/>
     </row>
-    <row r="5" spans="1:18" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="K5" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="L5" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="M5" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="O5" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="P5" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q5" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="R5" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="18"/>
-      <c r="M6" s="18"/>
-      <c r="N6" s="18"/>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="4"/>
-      <c r="P7" s="4"/>
-      <c r="Q7" s="4"/>
-      <c r="R7" s="4"/>
     </row>
-    <row r="8" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="17" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="18" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="19" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="20" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="O1:R1"/>
-    <mergeCell ref="O2:R2"/>
-    <mergeCell ref="A6:N6"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="K1:N1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="K2:N2"/>
-    <mergeCell ref="G1:J1"/>
-    <mergeCell ref="G2:J2"/>
+  <mergeCells count="2">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B2:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -1092,74 +838,74 @@
     <row r="1" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="6"/>
       <c r="B1" s="10" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D24" s="13" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1172,15 +918,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="ddfcbff1-988c-4780-af66-42272a7444f2" xsi:nil="true"/>
@@ -1196,6 +933,15 @@
     </SharedWithUsers>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1454,14 +1200,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{21273CB7-CC8A-48C1-BA2A-0CD67C70C578}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C6CC26F4-9ACA-496B-B719-4372C9693134}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="5eab2033-26a9-4886-8f5a-efa3f46bf7e3"/>
@@ -1474,6 +1212,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{21273CB7-CC8A-48C1-BA2A-0CD67C70C578}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Updated MIPI_deployment.xlsx from unstable branch
</commit_message>
<xml_diff>
--- a/MIPI_deployment.xlsx
+++ b/MIPI_deployment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\home\germaine\work\external_drive\jetson\l4t_eg\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cyril.germaine\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F34239B7-3CD0-43C9-86A0-DA429DC43A3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{944E98FE-0335-4CCC-B6DD-B0A810DF6A8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="360" windowWidth="25440" windowHeight="15390" activeTab="1" xr2:uid="{D61E0E21-A3C2-41B9-A323-5A81E21B33EC}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{D61E0E21-A3C2-41B9-A323-5A81E21B33EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Jetson" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="40">
   <si>
     <t>System On Module</t>
   </si>
@@ -82,10 +82,6 @@
   <si>
     <t>JetPack 5.1.3
 L4T 35.5.0</t>
-  </si>
-  <si>
-    <t>JetPack 6.0
-L4T 36.3</t>
   </si>
   <si>
     <t>Dione 640/1280</t>
@@ -115,13 +111,6 @@
   </si>
   <si>
     <t>* GitHub repo for Yocto : https://github.com/xenicsir/dione_mipi_tegra/tree/main/yocto</t>
-  </si>
-  <si>
-    <t>Jetson Xavier</t>
-  </si>
-  <si>
-    <t>Jetson AGX Orin
-Auvidea X230D</t>
   </si>
   <si>
     <t>CSI Connector type</t>
@@ -163,6 +152,30 @@
   </si>
   <si>
     <t>Not supported</t>
+  </si>
+  <si>
+    <t>Jetson Orin NX devkit</t>
+  </si>
+  <si>
+    <t>Jetson Xavier NX devkit</t>
+  </si>
+  <si>
+    <t>Jetson Nano devkit</t>
+  </si>
+  <si>
+    <t>Jetson AGX Orin /
+Auvidea X230D carrier board</t>
+  </si>
+  <si>
+    <t>Jetson Orin NX</t>
+  </si>
+  <si>
+    <t>JetPack 6.2
+L4T 36.4.3</t>
+  </si>
+  <si>
+    <t>- Waveshare JETSON-ORIN-NX-DEV-KIT
+- Nvidia Orin Nano devkit</t>
   </si>
 </sst>
 </file>
@@ -281,9 +294,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -296,17 +306,20 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -338,7 +351,7 @@
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>86898</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>172133</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -736,10 +749,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B889CEB-6ACC-47C4-9199-C4DCCE542BFC}">
-  <dimension ref="A1:N20"/>
+  <dimension ref="A1:R20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -750,78 +763,92 @@
     <col min="4" max="4" width="10" style="1" customWidth="1"/>
     <col min="5" max="5" width="7.5703125" style="1" customWidth="1"/>
     <col min="6" max="6" width="8" style="1" customWidth="1"/>
-    <col min="7" max="8" width="7.5703125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="7.28515625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="7.5703125" style="1" customWidth="1"/>
     <col min="9" max="10" width="7.7109375" style="1" customWidth="1"/>
     <col min="11" max="11" width="8.42578125" style="1" customWidth="1"/>
     <col min="12" max="12" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="8.28515625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="10.85546875" style="1" customWidth="1"/>
-    <col min="15" max="15" width="8" style="1" customWidth="1"/>
-    <col min="16" max="16" width="11" style="1" customWidth="1"/>
-    <col min="17" max="17" width="13.85546875" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="11.42578125" style="1"/>
+    <col min="14" max="14" width="8.85546875" style="1" customWidth="1"/>
+    <col min="15" max="15" width="8.42578125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.28515625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="8.85546875" style="1" customWidth="1"/>
+    <col min="19" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17" t="s">
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17" t="s">
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15"/>
+      <c r="R1" s="15"/>
     </row>
-    <row r="2" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17" t="s">
+      <c r="B2" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="L2" s="17"/>
-      <c r="M2" s="17"/>
-      <c r="N2" s="17"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="15"/>
+      <c r="R2" s="15"/>
     </row>
-    <row r="3" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>7</v>
@@ -851,116 +878,152 @@
         <v>12</v>
       </c>
       <c r="N3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>13</v>
       </c>
+      <c r="B4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="R4" s="5" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="4" spans="1:14" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="5" t="s">
+    <row r="5" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="K4" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="L4" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="M4" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>35</v>
+      <c r="B5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="R5" s="5" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="K5" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="L5" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="M5" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>35</v>
-      </c>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="18"/>
+      <c r="M6" s="18"/>
+      <c r="N6" s="18"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="16"/>
-      <c r="L6" s="16"/>
-      <c r="M6" s="16"/>
-      <c r="N6" s="16"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -975,22 +1038,28 @@
       <c r="L7" s="4"/>
       <c r="M7" s="4"/>
       <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="4"/>
+      <c r="R7" s="4"/>
     </row>
-    <row r="8" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="17" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="18" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="19" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="20" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="9">
+    <mergeCell ref="O1:R1"/>
+    <mergeCell ref="O2:R2"/>
     <mergeCell ref="A6:N6"/>
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="K1:N1"/>
@@ -1008,75 +1077,89 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DCCCDB1-1EA5-4151-AA8C-0720347F41D2}">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" style="13" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" style="14" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" style="12" customWidth="1"/>
     <col min="3" max="3" width="21.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="6"/>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="D1" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="7" t="s">
+    </row>
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>28</v>
       </c>
+      <c r="D4" s="8" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="C5" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>26</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="24" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D24" s="14" t="s">
-        <v>32</v>
+      <c r="D24" s="13" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1098,6 +1181,24 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="ddfcbff1-988c-4780-af66-42272a7444f2" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5eab2033-26a9-4886-8f5a-efa3f46bf7e3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <SharedWithUsers xmlns="ddfcbff1-988c-4780-af66-42272a7444f2">
+      <UserInfo>
+        <DisplayName>Cyril Germaine</DisplayName>
+        <AccountId>370</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100994F61C2E354C24B867AAD14EB9B712B" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="173ead120da22e4d04d58d9334952390">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5eab2033-26a9-4886-8f5a-efa3f46bf7e3" xmlns:ns3="ddfcbff1-988c-4780-af66-42272a7444f2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7ed80a0b9a34c83decd038c2f8c861fc" ns2:_="" ns3:_="">
     <xsd:import namespace="5eab2033-26a9-4886-8f5a-efa3f46bf7e3"/>
@@ -1352,24 +1453,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="ddfcbff1-988c-4780-af66-42272a7444f2" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5eab2033-26a9-4886-8f5a-efa3f46bf7e3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <SharedWithUsers xmlns="ddfcbff1-988c-4780-af66-42272a7444f2">
-      <UserInfo>
-        <DisplayName>Cyril Germaine</DisplayName>
-        <AccountId>370</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{21273CB7-CC8A-48C1-BA2A-0CD67C70C578}">
   <ds:schemaRefs>
@@ -1379,6 +1462,23 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C6CC26F4-9ACA-496B-B719-4372C9693134}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="5eab2033-26a9-4886-8f5a-efa3f46bf7e3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="ddfcbff1-988c-4780-af66-42272a7444f2"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31B71CDC-0E86-4889-96FE-F63C9CD1A6C7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1395,21 +1495,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C6CC26F4-9ACA-496B-B719-4372C9693134}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="5eab2033-26a9-4886-8f5a-efa3f46bf7e3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="ddfcbff1-988c-4780-af66-42272a7444f2"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added drivers for Forecr DSBOARD ORNXS L4T 36.4.3 and 36.4.4
</commit_message>
<xml_diff>
--- a/MIPI_deployment.xlsx
+++ b/MIPI_deployment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cyril.germaine\Documents\work\projets\MIPI\mipi_l4t_eg_main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EFB20DE-FC43-4F99-A52A-3C038A09F4D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8E117A6-B04F-4C0B-9E7F-5B6BE739FD34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{D61E0E21-A3C2-41B9-A323-5A81E21B33EC}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="49">
   <si>
     <t>Jetson Nano</t>
   </si>
@@ -203,6 +203,9 @@
   </si>
   <si>
     <t>Can Not Be Supported</t>
+  </si>
+  <si>
+    <t>download</t>
   </si>
 </sst>
 </file>
@@ -449,7 +452,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -558,7 +561,7 @@
         </ext>
       </extLst>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <extLst>
         <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
@@ -566,7 +569,7 @@
         </ext>
       </extLst>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <extLst>
         <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
@@ -574,7 +577,7 @@
         </ext>
       </extLst>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <extLst>
         <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
@@ -582,7 +585,7 @@
         </ext>
       </extLst>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <extLst>
         <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
@@ -590,7 +593,7 @@
         </ext>
       </extLst>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <extLst>
         <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
@@ -598,7 +601,7 @@
         </ext>
       </extLst>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <extLst>
         <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
@@ -606,7 +609,7 @@
         </ext>
       </extLst>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <extLst>
         <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
@@ -614,7 +617,7 @@
         </ext>
       </extLst>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <extLst>
         <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
@@ -622,7 +625,7 @@
         </ext>
       </extLst>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <extLst>
         <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
@@ -630,7 +633,7 @@
         </ext>
       </extLst>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <extLst>
         <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
@@ -638,7 +641,13 @@
         </ext>
       </extLst>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <extLst>
         <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
@@ -646,13 +655,22 @@
         </ext>
       </extLst>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <extLst>
         <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
@@ -660,22 +678,7 @@
         </ext>
       </extLst>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <extLst>
         <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
@@ -683,7 +686,7 @@
         </ext>
       </extLst>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <extLst>
         <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
@@ -691,7 +694,7 @@
         </ext>
       </extLst>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <extLst>
         <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
@@ -699,7 +702,20 @@
         </ext>
       </extLst>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <extLst>
         <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
@@ -707,7 +723,43 @@
         </ext>
       </extLst>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <extLst>
         <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
@@ -715,20 +767,82 @@
         </ext>
       </extLst>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <extLst>
         <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
@@ -736,43 +850,7 @@
         </ext>
       </extLst>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <extLst>
         <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
@@ -780,18 +858,10 @@
         </ext>
       </extLst>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <extLst>
-        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
-          <xfpb:xfComplement i="0"/>
-        </ext>
-      </extLst>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -806,95 +876,7 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <extLst>
-        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
-          <xfpb:xfComplement i="0"/>
-        </ext>
-      </extLst>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <extLst>
-        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
-          <xfpb:xfComplement i="0"/>
-        </ext>
-      </extLst>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1348,7 +1330,7 @@
       <pane xSplit="1" ySplit="5" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="R16" sqref="R16"/>
+      <selection pane="bottomRight" activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1381,196 +1363,196 @@
       <c r="A1" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="85" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="85"/>
-      <c r="D1" s="85"/>
-      <c r="E1" s="85"/>
-      <c r="F1" s="89" t="s">
+      <c r="B1" s="80" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="84" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="89"/>
-      <c r="H1" s="89"/>
-      <c r="I1" s="89"/>
-      <c r="J1" s="93" t="s">
-        <v>1</v>
-      </c>
-      <c r="K1" s="93"/>
-      <c r="L1" s="93"/>
-      <c r="M1" s="93"/>
-      <c r="N1" s="97" t="s">
+      <c r="G1" s="84"/>
+      <c r="H1" s="84"/>
+      <c r="I1" s="84"/>
+      <c r="J1" s="67" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" s="67"/>
+      <c r="L1" s="67"/>
+      <c r="M1" s="67"/>
+      <c r="N1" s="71" t="s">
         <v>34</v>
       </c>
-      <c r="O1" s="97"/>
-      <c r="P1" s="97"/>
-      <c r="Q1" s="97"/>
-      <c r="R1" s="97"/>
-      <c r="S1" s="97"/>
-      <c r="T1" s="97"/>
-      <c r="U1" s="97"/>
+      <c r="O1" s="71"/>
+      <c r="P1" s="71"/>
+      <c r="Q1" s="71"/>
+      <c r="R1" s="71"/>
+      <c r="S1" s="71"/>
+      <c r="T1" s="71"/>
+      <c r="U1" s="71"/>
     </row>
     <row r="2" spans="1:21" ht="46.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="86" t="s">
+      <c r="B2" s="81" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="87"/>
-      <c r="D2" s="87"/>
-      <c r="E2" s="88"/>
-      <c r="F2" s="90" t="s">
+      <c r="C2" s="82"/>
+      <c r="D2" s="82"/>
+      <c r="E2" s="83"/>
+      <c r="F2" s="85" t="s">
         <v>43</v>
       </c>
-      <c r="G2" s="91"/>
-      <c r="H2" s="91"/>
-      <c r="I2" s="92"/>
-      <c r="J2" s="94" t="s">
+      <c r="G2" s="86"/>
+      <c r="H2" s="86"/>
+      <c r="I2" s="87"/>
+      <c r="J2" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="K2" s="95"/>
-      <c r="L2" s="95"/>
-      <c r="M2" s="96"/>
-      <c r="N2" s="98" t="s">
+      <c r="K2" s="69"/>
+      <c r="L2" s="69"/>
+      <c r="M2" s="70"/>
+      <c r="N2" s="72" t="s">
         <v>45</v>
       </c>
-      <c r="O2" s="99"/>
-      <c r="P2" s="99"/>
-      <c r="Q2" s="100"/>
-      <c r="R2" s="98" t="s">
+      <c r="O2" s="73"/>
+      <c r="P2" s="73"/>
+      <c r="Q2" s="74"/>
+      <c r="R2" s="72" t="s">
         <v>46</v>
       </c>
-      <c r="S2" s="99"/>
-      <c r="T2" s="99"/>
-      <c r="U2" s="100"/>
+      <c r="S2" s="73"/>
+      <c r="T2" s="73"/>
+      <c r="U2" s="74"/>
     </row>
     <row r="3" spans="1:21" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="56"/>
-      <c r="B3" s="58"/>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="59"/>
-      <c r="F3" s="62"/>
-      <c r="G3" s="52"/>
-      <c r="H3" s="52"/>
-      <c r="I3" s="63"/>
-      <c r="J3" s="58"/>
-      <c r="K3" s="51"/>
-      <c r="L3" s="51"/>
-      <c r="M3" s="59"/>
-      <c r="N3" s="58"/>
-      <c r="O3" s="51"/>
-      <c r="P3" s="51"/>
-      <c r="Q3" s="59"/>
-      <c r="R3" s="58"/>
-      <c r="S3" s="51"/>
-      <c r="T3" s="51"/>
-      <c r="U3" s="59"/>
+      <c r="A3" s="54"/>
+      <c r="B3" s="56"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="60"/>
+      <c r="G3" s="50"/>
+      <c r="H3" s="50"/>
+      <c r="I3" s="61"/>
+      <c r="J3" s="56"/>
+      <c r="K3" s="49"/>
+      <c r="L3" s="49"/>
+      <c r="M3" s="57"/>
+      <c r="N3" s="56"/>
+      <c r="O3" s="49"/>
+      <c r="P3" s="49"/>
+      <c r="Q3" s="57"/>
+      <c r="R3" s="56"/>
+      <c r="S3" s="49"/>
+      <c r="T3" s="49"/>
+      <c r="U3" s="57"/>
     </row>
     <row r="4" spans="1:21" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="81" t="s">
+      <c r="A4" s="75" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="79" t="s">
+      <c r="B4" s="93" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="80"/>
-      <c r="D4" s="80" t="s">
+      <c r="C4" s="76"/>
+      <c r="D4" s="76" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="82" t="s">
+      <c r="E4" s="77" t="s">
         <v>27</v>
       </c>
-      <c r="F4" s="83" t="s">
+      <c r="F4" s="78" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="84"/>
-      <c r="H4" s="74" t="s">
+      <c r="G4" s="79"/>
+      <c r="H4" s="88" t="s">
         <v>26</v>
       </c>
-      <c r="I4" s="75" t="s">
+      <c r="I4" s="89" t="s">
         <v>27</v>
       </c>
-      <c r="J4" s="76" t="s">
+      <c r="J4" s="90" t="s">
         <v>25</v>
       </c>
-      <c r="K4" s="77"/>
-      <c r="L4" s="78" t="s">
+      <c r="K4" s="91"/>
+      <c r="L4" s="92" t="s">
         <v>26</v>
       </c>
-      <c r="M4" s="72" t="s">
+      <c r="M4" s="96" t="s">
         <v>27</v>
       </c>
-      <c r="N4" s="73" t="s">
+      <c r="N4" s="97" t="s">
         <v>25</v>
       </c>
-      <c r="O4" s="70"/>
-      <c r="P4" s="70" t="s">
+      <c r="O4" s="94"/>
+      <c r="P4" s="94" t="s">
         <v>26</v>
       </c>
-      <c r="Q4" s="71" t="s">
+      <c r="Q4" s="95" t="s">
         <v>27</v>
       </c>
-      <c r="R4" s="73" t="s">
+      <c r="R4" s="97" t="s">
         <v>25</v>
       </c>
-      <c r="S4" s="70"/>
-      <c r="T4" s="70" t="s">
+      <c r="S4" s="94"/>
+      <c r="T4" s="94" t="s">
         <v>26</v>
       </c>
-      <c r="U4" s="71" t="s">
+      <c r="U4" s="95" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="81"/>
-      <c r="B5" s="36" t="s">
+      <c r="A5" s="75"/>
+      <c r="B5" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="54" t="s">
+      <c r="C5" s="52" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="80"/>
-      <c r="E5" s="82"/>
-      <c r="F5" s="44" t="s">
+      <c r="D5" s="76"/>
+      <c r="E5" s="77"/>
+      <c r="F5" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="G5" s="55" t="s">
+      <c r="G5" s="53" t="s">
         <v>39</v>
       </c>
-      <c r="H5" s="74"/>
-      <c r="I5" s="75"/>
-      <c r="J5" s="45" t="s">
+      <c r="H5" s="88"/>
+      <c r="I5" s="89"/>
+      <c r="J5" s="43" t="s">
         <v>38</v>
       </c>
-      <c r="K5" s="53" t="s">
+      <c r="K5" s="51" t="s">
         <v>39</v>
       </c>
-      <c r="L5" s="78"/>
-      <c r="M5" s="72"/>
-      <c r="N5" s="46" t="s">
+      <c r="L5" s="92"/>
+      <c r="M5" s="96"/>
+      <c r="N5" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="O5" s="47" t="s">
+      <c r="O5" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="P5" s="70"/>
-      <c r="Q5" s="71"/>
-      <c r="R5" s="46" t="s">
+      <c r="P5" s="94"/>
+      <c r="Q5" s="95"/>
+      <c r="R5" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="S5" s="47" t="s">
+      <c r="S5" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="T5" s="70"/>
-      <c r="U5" s="71"/>
+      <c r="T5" s="94"/>
+      <c r="U5" s="95"/>
     </row>
     <row r="6" spans="1:21" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="37" t="b">
+      <c r="B6" s="36" t="b">
         <v>1</v>
       </c>
       <c r="C6" s="12" t="b">
@@ -1579,10 +1561,10 @@
       <c r="D6" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="60" t="s">
+      <c r="E6" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="30" t="b">
+      <c r="F6" s="29" t="b">
         <v>0</v>
       </c>
       <c r="G6" s="15" t="b">
@@ -1591,10 +1573,10 @@
       <c r="H6" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="I6" s="31" t="s">
-        <v>29</v>
-      </c>
-      <c r="J6" s="25" t="s">
+      <c r="I6" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="J6" s="24" t="s">
         <v>47</v>
       </c>
       <c r="K6" s="17" t="s">
@@ -1603,7 +1585,7 @@
       <c r="L6" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="M6" s="26" t="s">
+      <c r="M6" s="25" t="s">
         <v>29</v>
       </c>
       <c r="N6" s="20" t="s">
@@ -1632,10 +1614,10 @@
       </c>
     </row>
     <row r="7" spans="1:21" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="35" t="s">
+      <c r="A7" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="37" t="b">
+      <c r="B7" s="36" t="b">
         <v>1</v>
       </c>
       <c r="C7" s="12" t="b">
@@ -1644,10 +1626,10 @@
       <c r="D7" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="E7" s="60" t="s">
+      <c r="E7" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="F7" s="30" t="b">
+      <c r="F7" s="29" t="b">
         <v>0</v>
       </c>
       <c r="G7" s="15" t="b">
@@ -1656,10 +1638,10 @@
       <c r="H7" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="I7" s="31" t="s">
-        <v>29</v>
-      </c>
-      <c r="J7" s="25" t="s">
+      <c r="I7" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="J7" s="24" t="s">
         <v>47</v>
       </c>
       <c r="K7" s="17" t="s">
@@ -1668,7 +1650,7 @@
       <c r="L7" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="M7" s="26" t="s">
+      <c r="M7" s="25" t="s">
         <v>29</v>
       </c>
       <c r="N7" s="20" t="s">
@@ -1697,10 +1679,10 @@
       </c>
     </row>
     <row r="8" spans="1:21" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="35" t="s">
+      <c r="A8" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="37" t="b">
+      <c r="B8" s="36" t="b">
         <v>1</v>
       </c>
       <c r="C8" s="12" t="b">
@@ -1709,10 +1691,10 @@
       <c r="D8" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="E8" s="60" t="s">
+      <c r="E8" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="F8" s="30" t="b">
+      <c r="F8" s="29" t="b">
         <v>0</v>
       </c>
       <c r="G8" s="15" t="b">
@@ -1721,10 +1703,10 @@
       <c r="H8" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="I8" s="31" t="s">
-        <v>29</v>
-      </c>
-      <c r="J8" s="25" t="s">
+      <c r="I8" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="J8" s="24" t="s">
         <v>47</v>
       </c>
       <c r="K8" s="17" t="s">
@@ -1733,7 +1715,7 @@
       <c r="L8" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="M8" s="26" t="s">
+      <c r="M8" s="25" t="s">
         <v>29</v>
       </c>
       <c r="N8" s="20" t="s">
@@ -1762,10 +1744,10 @@
       </c>
     </row>
     <row r="9" spans="1:21" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="57" t="s">
+      <c r="A9" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="37" t="b">
+      <c r="B9" s="36" t="b">
         <v>1</v>
       </c>
       <c r="C9" s="12" t="b">
@@ -1774,10 +1756,10 @@
       <c r="D9" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="E9" s="61" t="s">
-        <v>33</v>
-      </c>
-      <c r="F9" s="30" t="b">
+      <c r="E9" s="59" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" s="29" t="b">
         <v>0</v>
       </c>
       <c r="G9" s="15" t="b">
@@ -1786,10 +1768,10 @@
       <c r="H9" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="I9" s="31" t="s">
-        <v>29</v>
-      </c>
-      <c r="J9" s="25" t="s">
+      <c r="I9" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="J9" s="24" t="s">
         <v>47</v>
       </c>
       <c r="K9" s="17" t="s">
@@ -1798,7 +1780,7 @@
       <c r="L9" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="M9" s="26" t="s">
+      <c r="M9" s="25" t="s">
         <v>29</v>
       </c>
       <c r="N9" s="20" t="s">
@@ -1827,10 +1809,10 @@
       </c>
     </row>
     <row r="10" spans="1:21" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="57" t="s">
+      <c r="A10" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="37" t="b">
+      <c r="B10" s="36" t="b">
         <v>1</v>
       </c>
       <c r="C10" s="12" t="b">
@@ -1839,10 +1821,10 @@
       <c r="D10" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="E10" s="61" t="s">
-        <v>33</v>
-      </c>
-      <c r="F10" s="30" t="b">
+      <c r="E10" s="59" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" s="29" t="b">
         <v>0</v>
       </c>
       <c r="G10" s="15" t="b">
@@ -1851,10 +1833,10 @@
       <c r="H10" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="I10" s="31" t="s">
-        <v>29</v>
-      </c>
-      <c r="J10" s="25" t="s">
+      <c r="I10" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="J10" s="24" t="s">
         <v>47</v>
       </c>
       <c r="K10" s="17" t="s">
@@ -1863,7 +1845,7 @@
       <c r="L10" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="M10" s="26" t="s">
+      <c r="M10" s="25" t="s">
         <v>29</v>
       </c>
       <c r="N10" s="20" t="s">
@@ -1892,10 +1874,10 @@
       </c>
     </row>
     <row r="11" spans="1:21" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="57" t="s">
+      <c r="A11" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="38" t="s">
+      <c r="B11" s="37" t="s">
         <v>47</v>
       </c>
       <c r="C11" s="14" t="s">
@@ -1904,10 +1886,10 @@
       <c r="D11" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E11" s="39" t="s">
-        <v>29</v>
-      </c>
-      <c r="F11" s="30" t="b">
+      <c r="E11" s="38" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" s="29" t="b">
         <v>1</v>
       </c>
       <c r="G11" s="15" t="b">
@@ -1916,10 +1898,10 @@
       <c r="H11" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="I11" s="64" t="s">
-        <v>33</v>
-      </c>
-      <c r="J11" s="25" t="b">
+      <c r="I11" s="62" t="s">
+        <v>48</v>
+      </c>
+      <c r="J11" s="24" t="b">
         <v>0</v>
       </c>
       <c r="K11" s="17" t="b">
@@ -1928,7 +1910,7 @@
       <c r="L11" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="M11" s="26" t="s">
+      <c r="M11" s="25" t="s">
         <v>29</v>
       </c>
       <c r="N11" s="20" t="s">
@@ -1957,10 +1939,10 @@
       </c>
     </row>
     <row r="12" spans="1:21" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="57" t="s">
+      <c r="A12" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="38" t="s">
+      <c r="B12" s="37" t="s">
         <v>47</v>
       </c>
       <c r="C12" s="14" t="s">
@@ -1969,10 +1951,10 @@
       <c r="D12" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E12" s="39" t="s">
-        <v>29</v>
-      </c>
-      <c r="F12" s="30" t="b">
+      <c r="E12" s="38" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12" s="29" t="b">
         <v>1</v>
       </c>
       <c r="G12" s="15" t="b">
@@ -1981,10 +1963,10 @@
       <c r="H12" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="I12" s="64" t="s">
-        <v>33</v>
-      </c>
-      <c r="J12" s="25" t="b">
+      <c r="I12" s="62" t="s">
+        <v>48</v>
+      </c>
+      <c r="J12" s="24" t="b">
         <v>1</v>
       </c>
       <c r="K12" s="17" t="b">
@@ -1993,7 +1975,7 @@
       <c r="L12" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="M12" s="65" t="s">
+      <c r="M12" s="63" t="s">
         <v>33</v>
       </c>
       <c r="N12" s="20" t="b">
@@ -2022,10 +2004,10 @@
       </c>
     </row>
     <row r="13" spans="1:21" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="57" t="s">
+      <c r="A13" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="38" t="s">
+      <c r="B13" s="37" t="s">
         <v>47</v>
       </c>
       <c r="C13" s="14" t="s">
@@ -2034,10 +2016,10 @@
       <c r="D13" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="39" t="s">
-        <v>29</v>
-      </c>
-      <c r="F13" s="30" t="b">
+      <c r="E13" s="38" t="s">
+        <v>29</v>
+      </c>
+      <c r="F13" s="29" t="b">
         <v>1</v>
       </c>
       <c r="G13" s="15" t="b">
@@ -2046,10 +2028,10 @@
       <c r="H13" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="I13" s="64" t="s">
-        <v>33</v>
-      </c>
-      <c r="J13" s="25" t="b">
+      <c r="I13" s="62" t="s">
+        <v>48</v>
+      </c>
+      <c r="J13" s="24" t="b">
         <v>1</v>
       </c>
       <c r="K13" s="17" t="b">
@@ -2058,7 +2040,7 @@
       <c r="L13" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="M13" s="65" t="s">
+      <c r="M13" s="63" t="s">
         <v>33</v>
       </c>
       <c r="N13" s="20" t="b">
@@ -2087,10 +2069,10 @@
       </c>
     </row>
     <row r="14" spans="1:21" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="57" t="s">
+      <c r="A14" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="38" t="s">
+      <c r="B14" s="37" t="s">
         <v>47</v>
       </c>
       <c r="C14" s="14" t="s">
@@ -2099,10 +2081,10 @@
       <c r="D14" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E14" s="39" t="s">
-        <v>29</v>
-      </c>
-      <c r="F14" s="30" t="b">
+      <c r="E14" s="38" t="s">
+        <v>29</v>
+      </c>
+      <c r="F14" s="29" t="b">
         <v>1</v>
       </c>
       <c r="G14" s="15" t="b">
@@ -2111,10 +2093,10 @@
       <c r="H14" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="I14" s="64" t="s">
-        <v>33</v>
-      </c>
-      <c r="J14" s="25" t="b">
+      <c r="I14" s="62" t="s">
+        <v>48</v>
+      </c>
+      <c r="J14" s="24" t="b">
         <v>1</v>
       </c>
       <c r="K14" s="17" t="b">
@@ -2123,7 +2105,7 @@
       <c r="L14" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="M14" s="65" t="s">
+      <c r="M14" s="63" t="s">
         <v>33</v>
       </c>
       <c r="N14" s="20" t="b">
@@ -2152,10 +2134,10 @@
       </c>
     </row>
     <row r="15" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="57" t="s">
+      <c r="A15" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="38" t="s">
+      <c r="B15" s="37" t="s">
         <v>47</v>
       </c>
       <c r="C15" s="14" t="s">
@@ -2164,10 +2146,10 @@
       <c r="D15" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E15" s="39" t="s">
-        <v>29</v>
-      </c>
-      <c r="F15" s="30" t="b">
+      <c r="E15" s="38" t="s">
+        <v>29</v>
+      </c>
+      <c r="F15" s="29" t="b">
         <v>0</v>
       </c>
       <c r="G15" s="15" t="b">
@@ -2176,10 +2158,10 @@
       <c r="H15" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="I15" s="31" t="s">
-        <v>29</v>
-      </c>
-      <c r="J15" s="25" t="b">
+      <c r="I15" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="J15" s="24" t="b">
         <v>0</v>
       </c>
       <c r="K15" s="17" t="b">
@@ -2188,7 +2170,7 @@
       <c r="L15" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="M15" s="26" t="s">
+      <c r="M15" s="25" t="s">
         <v>29</v>
       </c>
       <c r="N15" s="20" t="b">
@@ -2197,30 +2179,30 @@
       <c r="O15" s="19" t="b">
         <v>1</v>
       </c>
-      <c r="P15" s="43" t="s">
+      <c r="P15" s="98" t="s">
         <v>33</v>
       </c>
-      <c r="Q15" s="66" t="s">
+      <c r="Q15" s="64" t="s">
+        <v>48</v>
+      </c>
+      <c r="R15" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="S15" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="T15" s="98" t="s">
         <v>33</v>
       </c>
-      <c r="R15" s="20" t="b">
-        <v>1</v>
-      </c>
-      <c r="S15" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="T15" s="43" t="s">
-        <v>33</v>
-      </c>
-      <c r="U15" s="66" t="s">
-        <v>33</v>
+      <c r="U15" s="64" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="57" t="s">
+      <c r="A16" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="38" t="s">
+      <c r="B16" s="37" t="s">
         <v>47</v>
       </c>
       <c r="C16" s="14" t="s">
@@ -2229,10 +2211,10 @@
       <c r="D16" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E16" s="39" t="s">
-        <v>29</v>
-      </c>
-      <c r="F16" s="30" t="b">
+      <c r="E16" s="38" t="s">
+        <v>29</v>
+      </c>
+      <c r="F16" s="29" t="b">
         <v>0</v>
       </c>
       <c r="G16" s="15" t="b">
@@ -2241,10 +2223,10 @@
       <c r="H16" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="I16" s="31" t="s">
-        <v>29</v>
-      </c>
-      <c r="J16" s="25" t="b">
+      <c r="I16" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="J16" s="24" t="b">
         <v>0</v>
       </c>
       <c r="K16" s="17" t="b">
@@ -2253,7 +2235,7 @@
       <c r="L16" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="M16" s="26" t="s">
+      <c r="M16" s="25" t="s">
         <v>29</v>
       </c>
       <c r="N16" s="20" t="b">
@@ -2262,63 +2244,63 @@
       <c r="O16" s="19" t="b">
         <v>1</v>
       </c>
-      <c r="P16" s="43" t="s">
+      <c r="P16" s="98" t="s">
         <v>33</v>
       </c>
-      <c r="Q16" s="68" t="s">
+      <c r="Q16" s="65" t="s">
+        <v>48</v>
+      </c>
+      <c r="R16" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="S16" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="T16" s="98" t="s">
         <v>33</v>
       </c>
-      <c r="R16" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="S16" s="19" t="b">
-        <v>0</v>
-      </c>
-      <c r="T16" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="U16" s="21" t="s">
-        <v>29</v>
+      <c r="U16" s="65" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:21" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="57" t="s">
+      <c r="A17" s="55" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="C17" s="41" t="s">
-        <v>47</v>
-      </c>
-      <c r="D17" s="41" t="s">
-        <v>29</v>
-      </c>
-      <c r="E17" s="42" t="s">
-        <v>29</v>
-      </c>
-      <c r="F17" s="32" t="b">
-        <v>0</v>
-      </c>
-      <c r="G17" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="H17" s="33" t="s">
-        <v>29</v>
-      </c>
-      <c r="I17" s="34" t="s">
-        <v>29</v>
-      </c>
-      <c r="J17" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="K17" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="L17" s="28" t="s">
-        <v>29</v>
-      </c>
-      <c r="M17" s="29" t="s">
+      <c r="B17" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="40" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17" s="41" t="s">
+        <v>29</v>
+      </c>
+      <c r="F17" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="G17" s="32" t="b">
+        <v>0</v>
+      </c>
+      <c r="H17" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="I17" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="J17" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="K17" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="L17" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="M17" s="28" t="s">
         <v>29</v>
       </c>
       <c r="N17" s="22" t="b">
@@ -2327,42 +2309,47 @@
       <c r="O17" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="P17" s="67" t="s">
+      <c r="P17" s="98" t="s">
         <v>33</v>
       </c>
-      <c r="Q17" s="69" t="s">
+      <c r="Q17" s="66" t="s">
+        <v>48</v>
+      </c>
+      <c r="R17" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="S17" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="T17" s="98" t="s">
         <v>33</v>
       </c>
-      <c r="R17" s="22" t="b">
-        <v>0</v>
-      </c>
-      <c r="S17" s="23" t="b">
-        <v>0</v>
-      </c>
-      <c r="T17" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="U17" s="24" t="s">
-        <v>29</v>
+      <c r="U17" s="66" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="19" spans="1:21" ht="60" x14ac:dyDescent="0.25">
-      <c r="A19" s="48" t="s">
+      <c r="A19" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="B19" s="50" t="s">
+      <c r="B19" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="49"/>
+      <c r="C19" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="J1:M1"/>
-    <mergeCell ref="J2:M2"/>
-    <mergeCell ref="N1:U1"/>
-    <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="R2:U2"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="L4:L5"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="T4:T5"/>
+    <mergeCell ref="U4:U5"/>
+    <mergeCell ref="M4:M5"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="Q4:Q5"/>
+    <mergeCell ref="R4:S4"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="D4:D5"/>
     <mergeCell ref="E4:E5"/>
@@ -2373,16 +2360,11 @@
     <mergeCell ref="F2:I2"/>
     <mergeCell ref="H4:H5"/>
     <mergeCell ref="I4:I5"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="L4:L5"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="T4:T5"/>
-    <mergeCell ref="U4:U5"/>
-    <mergeCell ref="M4:M5"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="P4:P5"/>
-    <mergeCell ref="Q4:Q5"/>
-    <mergeCell ref="R4:S4"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="N1:U1"/>
+    <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="R2:U2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D6" r:id="rId1" xr:uid="{E221AAD3-4BB4-4EDE-B796-266DB5695C55}"/>
@@ -2405,16 +2387,20 @@
     <hyperlink ref="M13" r:id="rId18" xr:uid="{49AEE96E-2815-466A-9AD9-F1D10ACB5170}"/>
     <hyperlink ref="M14" r:id="rId19" xr:uid="{698C4CFD-83C5-4F55-91CC-ACE56352881D}"/>
     <hyperlink ref="B19" r:id="rId20" xr:uid="{A43DB891-0AA9-40A8-A009-27A37C73A6AE}"/>
-    <hyperlink ref="P15" r:id="rId21" xr:uid="{F21FAFB5-A511-4818-BD3E-958DE750FDDF}"/>
-    <hyperlink ref="P16" r:id="rId22" xr:uid="{CA885AF9-436B-497E-8747-8BF0A28BA601}"/>
-    <hyperlink ref="P17" r:id="rId23" xr:uid="{1644D2AA-FD42-4EB8-B2F5-4123AA4981F4}"/>
-    <hyperlink ref="T15" r:id="rId24" xr:uid="{9835FCE2-6E9A-4F83-81BA-E7C190B8A3F4}"/>
-    <hyperlink ref="Q15" r:id="rId25" xr:uid="{A820D219-2552-4F82-A3ED-5F08305A7493}"/>
-    <hyperlink ref="U15" r:id="rId26" xr:uid="{77856E80-3321-4396-A55F-FD54E87CC72B}"/>
-    <hyperlink ref="D7" r:id="rId27" xr:uid="{C4CB9B01-30A3-41DC-BFB3-25D40247C7DA}"/>
-    <hyperlink ref="D8" r:id="rId28" xr:uid="{502E863D-13AD-40C5-9B40-E71F9AE604D1}"/>
-    <hyperlink ref="Q16" r:id="rId29" xr:uid="{F836DE37-F8DB-410D-801A-F332B71C039E}"/>
-    <hyperlink ref="Q17" r:id="rId30" xr:uid="{1B267D2F-16CD-4B1D-855E-9B2A0C44FF75}"/>
+    <hyperlink ref="Q15" r:id="rId21" xr:uid="{A820D219-2552-4F82-A3ED-5F08305A7493}"/>
+    <hyperlink ref="U15" r:id="rId22" xr:uid="{77856E80-3321-4396-A55F-FD54E87CC72B}"/>
+    <hyperlink ref="D7" r:id="rId23" xr:uid="{C4CB9B01-30A3-41DC-BFB3-25D40247C7DA}"/>
+    <hyperlink ref="D8" r:id="rId24" xr:uid="{502E863D-13AD-40C5-9B40-E71F9AE604D1}"/>
+    <hyperlink ref="Q16" r:id="rId25" xr:uid="{F836DE37-F8DB-410D-801A-F332B71C039E}"/>
+    <hyperlink ref="Q17" r:id="rId26" xr:uid="{1B267D2F-16CD-4B1D-855E-9B2A0C44FF75}"/>
+    <hyperlink ref="P15" r:id="rId27" xr:uid="{977E82EE-05DB-4152-80DC-0F31947E862C}"/>
+    <hyperlink ref="P16" r:id="rId28" xr:uid="{020CA32C-74AC-467A-9C84-DDF89C0D6A85}"/>
+    <hyperlink ref="P17" r:id="rId29" xr:uid="{C9865ED3-82E4-4A4C-A0DB-133281108C17}"/>
+    <hyperlink ref="T15" r:id="rId30" xr:uid="{8DF6A1BC-9DB8-41D3-B138-0DC0AE3FE5CF}"/>
+    <hyperlink ref="T16" r:id="rId31" xr:uid="{FA945D65-971B-4E59-9DDE-0B7D47C473DB}"/>
+    <hyperlink ref="T17" r:id="rId32" xr:uid="{04C6CE1A-3953-4144-B3BF-5E8AE90F3CF7}"/>
+    <hyperlink ref="U16" r:id="rId33" xr:uid="{5FAA7D0D-C079-4DFE-BC65-F006D5A0A201}"/>
+    <hyperlink ref="U17" r:id="rId34" xr:uid="{9920C8E7-E4BF-4179-8D2F-AC533F77D63A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2519,33 +2505,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="ddfcbff1-988c-4780-af66-42272a7444f2" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5eab2033-26a9-4886-8f5a-efa3f46bf7e3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <SharedWithUsers xmlns="ddfcbff1-988c-4780-af66-42272a7444f2">
-      <UserInfo>
-        <DisplayName>Cyril Germaine</DisplayName>
-        <AccountId>370</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100994F61C2E354C24B867AAD14EB9B712B" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="173ead120da22e4d04d58d9334952390">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5eab2033-26a9-4886-8f5a-efa3f46bf7e3" xmlns:ns3="ddfcbff1-988c-4780-af66-42272a7444f2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7ed80a0b9a34c83decd038c2f8c861fc" ns2:_="" ns3:_="">
     <xsd:import namespace="5eab2033-26a9-4886-8f5a-efa3f46bf7e3"/>
@@ -2800,32 +2759,34 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C6CC26F4-9ACA-496B-B719-4372C9693134}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="5eab2033-26a9-4886-8f5a-efa3f46bf7e3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="ddfcbff1-988c-4780-af66-42272a7444f2"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{21273CB7-CC8A-48C1-BA2A-0CD67C70C578}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="ddfcbff1-988c-4780-af66-42272a7444f2" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5eab2033-26a9-4886-8f5a-efa3f46bf7e3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <SharedWithUsers xmlns="ddfcbff1-988c-4780-af66-42272a7444f2">
+      <UserInfo>
+        <DisplayName>Cyril Germaine</DisplayName>
+        <AccountId>370</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31B71CDC-0E86-4889-96FE-F63C9CD1A6C7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2842,4 +2803,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{21273CB7-CC8A-48C1-BA2A-0CD67C70C578}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C6CC26F4-9ACA-496B-B719-4372C9693134}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="5eab2033-26a9-4886-8f5a-efa3f46bf7e3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="ddfcbff1-988c-4780-af66-42272a7444f2"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>